<commit_message>
unit eighty eight - intermediate
</commit_message>
<xml_diff>
--- a/homework/86.xlsx
+++ b/homework/86.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <xr:revisionPtr revIDLastSave="196" documentId="13_ncr:1_{6397D056-7233-42F8-9329-AC4D59D3BBF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D4CBA53A-A0B6-4754-9BEF-2225E3592AF7}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="4560" windowWidth="19470" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>